<commit_message>
bug fix from a review on 19/07/12
</commit_message>
<xml_diff>
--- a/data/sample/ingredents_dummy_data.xlsx
+++ b/data/sample/ingredents_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workplace\sse2019-group5\data\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576AF6ED-FF53-4E51-BB4B-5DA426516EA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5642D674-4B59-4D34-8C0B-A0B6423DFF1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35520" yWindow="5010" windowWidth="18060" windowHeight="9165" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingredients" sheetId="3" r:id="rId1"/>
@@ -4797,7 +4797,7 @@
       </c>
       <c r="AC4">
         <f ca="1">INT(RANDBETWEEN(5,12)*10)*10</f>
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="AD4" t="str">
         <f>C4&amp;" "&amp;D4&amp;" "&amp;F4&amp;"kcal"</f>
@@ -48184,10 +48184,10 @@
   <dimension ref="A1:Q92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M116" sqref="M116"/>
+      <selection pane="bottomRight" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -48712,7 +48712,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
@@ -57798,7 +57798,7 @@
       </c>
       <c r="J23" s="20">
         <f t="shared" ca="1" si="3"/>
-        <v>800</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -59976,15 +59976,15 @@
       </c>
       <c r="C2">
         <f ca="1">INT(RAND()*202)</f>
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <f ca="1">INT(RAND()*202)</f>
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E2">
         <f ca="1">INT(RAND()*202)</f>
-        <v>195</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -59996,15 +59996,15 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:E31" ca="1" si="0">INT(RAND()*202)</f>
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -60016,15 +60016,15 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -60036,15 +60036,15 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -60056,15 +60056,15 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>149</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>107</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -60076,15 +60076,15 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>198</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -60096,15 +60096,15 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>151</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -60116,15 +60116,15 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -60136,15 +60136,15 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>154</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>118</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -60156,15 +60156,15 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>127</v>
+        <v>190</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -60176,15 +60176,15 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>137</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -60196,15 +60196,15 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>109</v>
+        <v>199</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -60216,15 +60216,15 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>201</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>166</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -60236,15 +60236,15 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>197</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -60256,15 +60256,15 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -60276,15 +60276,15 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>156</v>
+        <v>99</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -60296,15 +60296,15 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>199</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>130</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -60316,15 +60316,15 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -60336,15 +60336,15 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>101</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>111</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -60356,15 +60356,15 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>52</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>127</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -60376,15 +60376,15 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>192</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>191</v>
+        <v>121</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -60396,15 +60396,15 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>161</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -60416,15 +60416,15 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>177</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -60436,15 +60436,15 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -60456,15 +60456,15 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>150</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -60476,15 +60476,15 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>182</v>
+        <v>49</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>170</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>141</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -60496,15 +60496,15 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>126</v>
+        <v>9</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>197</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -60516,15 +60516,15 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>157</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -60536,15 +60536,15 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>196</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -60556,15 +60556,15 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>107</v>
+        <v>193</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>